<commit_message>
Correction de la comparaison
</commit_message>
<xml_diff>
--- a/master2/exoxml/devoir/out.xlsx
+++ b/master2/exoxml/devoir/out.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>vous</t>
   </si>
@@ -32,6 +32,9 @@
     <t>mon</t>
   </si>
   <si>
+    <t>missing annotation</t>
+  </si>
+  <si>
     <t>moi</t>
   </si>
   <si>
@@ -53,6 +56,9 @@
     <t>Je</t>
   </si>
   <si>
+    <t>e</t>
+  </si>
+  <si>
     <t>te</t>
   </si>
   <si>
@@ -87,6 +93,12 @@
   </si>
   <si>
     <t>J</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> je</t>
+  </si>
+  <si>
+    <t>ous</t>
   </si>
 </sst>
 </file>
@@ -455,7 +467,7 @@
         <v>1</v>
       </c>
       <c r="I1" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -513,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -542,7 +554,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -571,7 +583,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -600,7 +612,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -616,20 +628,8 @@
       <c r="D7" t="s">
         <v>1</v>
       </c>
-      <c r="E7" t="n">
-        <v>7799</v>
-      </c>
-      <c r="F7" t="n">
-        <v>7802</v>
-      </c>
-      <c r="G7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" t="b">
-        <v>1</v>
+      <c r="E7" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -658,7 +658,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -669,25 +669,13 @@
         <v>12625</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" t="n">
-        <v>12622</v>
-      </c>
-      <c r="F9" t="n">
-        <v>12625</v>
-      </c>
-      <c r="G9" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" t="b">
-        <v>1</v>
+      <c r="E9" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -703,20 +691,8 @@
       <c r="D10" t="s">
         <v>1</v>
       </c>
-      <c r="E10" t="n">
-        <v>12667</v>
-      </c>
-      <c r="F10" t="n">
-        <v>12670</v>
-      </c>
-      <c r="G10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" t="b">
-        <v>1</v>
+      <c r="E10" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -727,25 +703,13 @@
         <v>15911</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="E11" t="n">
-        <v>15909</v>
-      </c>
-      <c r="F11" t="n">
-        <v>15911</v>
-      </c>
-      <c r="G11" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" t="b">
-        <v>1</v>
+      <c r="E11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -761,20 +725,8 @@
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" t="n">
-        <v>16984</v>
-      </c>
-      <c r="F12" t="n">
-        <v>16988</v>
-      </c>
-      <c r="G12" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
+      <c r="E12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13">
@@ -785,7 +737,7 @@
         <v>17086</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
@@ -797,7 +749,7 @@
         <v>17086</v>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H13" t="s">
         <v>1</v>
@@ -814,25 +766,13 @@
         <v>17089</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
         <v>1</v>
       </c>
-      <c r="E14" t="n">
-        <v>17087</v>
-      </c>
-      <c r="F14" t="n">
-        <v>17089</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" t="b">
-        <v>1</v>
+      <c r="E14" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -843,25 +783,13 @@
         <v>17247</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
       </c>
-      <c r="E15" t="n">
-        <v>17245</v>
-      </c>
-      <c r="F15" t="n">
-        <v>17247</v>
-      </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" t="b">
-        <v>1</v>
+      <c r="E15" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -872,25 +800,13 @@
         <v>17301</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
       </c>
-      <c r="E16" t="n">
-        <v>17296</v>
-      </c>
-      <c r="F16" t="n">
-        <v>17301</v>
-      </c>
-      <c r="G16" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" t="b">
-        <v>1</v>
+      <c r="E16" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="17">
@@ -901,25 +817,13 @@
         <v>17433</v>
       </c>
       <c r="C17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
-      <c r="E17" t="n">
-        <v>17423</v>
-      </c>
-      <c r="F17" t="n">
-        <v>17433</v>
-      </c>
-      <c r="G17" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
+      <c r="E17" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -935,20 +839,8 @@
       <c r="D18" t="s">
         <v>1</v>
       </c>
-      <c r="E18" t="n">
-        <v>17795</v>
-      </c>
-      <c r="F18" t="n">
-        <v>17799</v>
-      </c>
-      <c r="G18" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" t="b">
-        <v>1</v>
+      <c r="E18" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19">
@@ -959,25 +851,13 @@
         <v>18156</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
       </c>
-      <c r="E19" t="n">
-        <v>18154</v>
-      </c>
-      <c r="F19" t="n">
-        <v>18156</v>
-      </c>
-      <c r="G19" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" t="b">
-        <v>1</v>
+      <c r="E19" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="20">
@@ -988,19 +868,19 @@
         <v>18741</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
       </c>
       <c r="E20" t="n">
-        <v>18739</v>
+        <v>18740</v>
       </c>
       <c r="F20" t="n">
         <v>18741</v>
       </c>
       <c r="G20" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="H20" t="s">
         <v>1</v>
@@ -1017,7 +897,7 @@
         <v>19580</v>
       </c>
       <c r="C21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
@@ -1029,7 +909,7 @@
         <v>19580</v>
       </c>
       <c r="G21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H21" t="s">
         <v>1</v>
@@ -1046,7 +926,7 @@
         <v>19658</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
@@ -1058,7 +938,7 @@
         <v>19658</v>
       </c>
       <c r="G22" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="H22" t="s">
         <v>1</v>
@@ -1104,25 +984,13 @@
         <v>19832</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
       </c>
-      <c r="E24" t="n">
-        <v>19829</v>
-      </c>
-      <c r="F24" t="n">
-        <v>19832</v>
-      </c>
-      <c r="G24" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1</v>
-      </c>
-      <c r="I24" t="b">
-        <v>1</v>
+      <c r="E24" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25">
@@ -1133,25 +1001,13 @@
         <v>19912</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
       </c>
-      <c r="E25" t="n">
-        <v>19910</v>
-      </c>
-      <c r="F25" t="n">
-        <v>19912</v>
-      </c>
-      <c r="G25" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" t="s">
-        <v>1</v>
-      </c>
-      <c r="I25" t="b">
-        <v>1</v>
+      <c r="E25" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26">
@@ -1162,25 +1018,13 @@
         <v>19982</v>
       </c>
       <c r="C26" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
-      <c r="E26" t="n">
-        <v>19981</v>
-      </c>
-      <c r="F26" t="n">
-        <v>19982</v>
-      </c>
-      <c r="G26" t="s">
-        <v>14</v>
-      </c>
-      <c r="H26" t="s">
-        <v>1</v>
-      </c>
-      <c r="I26" t="b">
-        <v>1</v>
+      <c r="E26" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="27">
@@ -1191,25 +1035,13 @@
         <v>20031</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
       </c>
-      <c r="E27" t="n">
-        <v>20030</v>
-      </c>
-      <c r="F27" t="n">
-        <v>20031</v>
-      </c>
-      <c r="G27" t="s">
-        <v>15</v>
-      </c>
-      <c r="H27" t="s">
-        <v>1</v>
-      </c>
-      <c r="I27" t="b">
-        <v>1</v>
+      <c r="E27" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="28">
@@ -1220,25 +1052,13 @@
         <v>20077</v>
       </c>
       <c r="C28" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
-      <c r="E28" t="n">
-        <v>20076</v>
-      </c>
-      <c r="F28" t="n">
-        <v>20077</v>
-      </c>
-      <c r="G28" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" t="s">
-        <v>1</v>
-      </c>
-      <c r="I28" t="b">
-        <v>1</v>
+      <c r="E28" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="29">
@@ -1249,25 +1069,13 @@
         <v>20193</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
-      <c r="E29" t="n">
-        <v>20192</v>
-      </c>
-      <c r="F29" t="n">
-        <v>20193</v>
-      </c>
-      <c r="G29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" t="s">
-        <v>1</v>
-      </c>
-      <c r="I29" t="b">
-        <v>1</v>
+      <c r="E29" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -1278,25 +1086,13 @@
         <v>20236</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
-      <c r="E30" t="n">
-        <v>20234</v>
-      </c>
-      <c r="F30" t="n">
-        <v>20236</v>
-      </c>
-      <c r="G30" t="s">
-        <v>7</v>
-      </c>
-      <c r="H30" t="s">
-        <v>1</v>
-      </c>
-      <c r="I30" t="b">
-        <v>1</v>
+      <c r="E30" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="31">
@@ -1307,25 +1103,13 @@
         <v>20290</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
       </c>
-      <c r="E31" t="n">
-        <v>20289</v>
-      </c>
-      <c r="F31" t="n">
-        <v>20290</v>
-      </c>
-      <c r="G31" t="s">
-        <v>14</v>
-      </c>
-      <c r="H31" t="s">
-        <v>1</v>
-      </c>
-      <c r="I31" t="b">
-        <v>1</v>
+      <c r="E31" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -1336,7 +1120,7 @@
         <v>20353</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
@@ -1348,7 +1132,7 @@
         <v>20353</v>
       </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="H32" t="s">
         <v>1</v>
@@ -1365,25 +1149,13 @@
         <v>20464</v>
       </c>
       <c r="C33" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
-      <c r="E33" t="n">
-        <v>20462</v>
-      </c>
-      <c r="F33" t="n">
-        <v>20464</v>
-      </c>
-      <c r="G33" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" t="s">
-        <v>1</v>
-      </c>
-      <c r="I33" t="b">
-        <v>1</v>
+      <c r="E33" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="34">
@@ -1394,25 +1166,13 @@
         <v>20543</v>
       </c>
       <c r="C34" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
-      <c r="E34" t="n">
-        <v>20541</v>
-      </c>
-      <c r="F34" t="n">
-        <v>20543</v>
-      </c>
-      <c r="G34" t="s">
-        <v>7</v>
-      </c>
-      <c r="H34" t="s">
-        <v>1</v>
-      </c>
-      <c r="I34" t="b">
-        <v>1</v>
+      <c r="E34" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -1423,7 +1183,7 @@
         <v>20604</v>
       </c>
       <c r="C35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
@@ -1435,7 +1195,7 @@
         <v>20604</v>
       </c>
       <c r="G35" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
         <v>1</v>
@@ -1452,7 +1212,7 @@
         <v>20969</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
@@ -1464,13 +1224,13 @@
         <v>20969</v>
       </c>
       <c r="G36" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H36" t="s">
         <v>1</v>
       </c>
       <c r="I36" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -1481,25 +1241,13 @@
         <v>21119</v>
       </c>
       <c r="C37" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
-      <c r="E37" t="n">
-        <v>21116</v>
-      </c>
-      <c r="F37" t="n">
-        <v>21119</v>
-      </c>
-      <c r="G37" t="s">
-        <v>18</v>
-      </c>
-      <c r="H37" t="s">
-        <v>1</v>
-      </c>
-      <c r="I37" t="b">
-        <v>1</v>
+      <c r="E37" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="38">
@@ -1510,25 +1258,13 @@
         <v>21264</v>
       </c>
       <c r="C38" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
-      <c r="E38" t="n">
-        <v>21260</v>
-      </c>
-      <c r="F38" t="n">
-        <v>21264</v>
-      </c>
-      <c r="G38" t="s">
-        <v>19</v>
-      </c>
-      <c r="H38" t="s">
-        <v>1</v>
-      </c>
-      <c r="I38" t="b">
-        <v>1</v>
+      <c r="E38" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -1539,25 +1275,13 @@
         <v>21823</v>
       </c>
       <c r="C39" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
-      <c r="E39" t="n">
-        <v>21819</v>
-      </c>
-      <c r="F39" t="n">
-        <v>21823</v>
-      </c>
-      <c r="G39" t="s">
-        <v>20</v>
-      </c>
-      <c r="H39" t="s">
-        <v>1</v>
-      </c>
-      <c r="I39" t="b">
-        <v>1</v>
+      <c r="E39" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -1568,25 +1292,13 @@
         <v>21899</v>
       </c>
       <c r="C40" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
-      <c r="E40" t="n">
-        <v>21895</v>
-      </c>
-      <c r="F40" t="n">
-        <v>21899</v>
-      </c>
-      <c r="G40" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" t="s">
-        <v>1</v>
-      </c>
-      <c r="I40" t="b">
-        <v>1</v>
+      <c r="E40" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="41">
@@ -1597,25 +1309,13 @@
         <v>21945</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
-      <c r="E41" t="n">
-        <v>21942</v>
-      </c>
-      <c r="F41" t="n">
-        <v>21945</v>
-      </c>
-      <c r="G41" t="s">
-        <v>21</v>
-      </c>
-      <c r="H41" t="s">
-        <v>1</v>
-      </c>
-      <c r="I41" t="b">
-        <v>1</v>
+      <c r="E41" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -1626,7 +1326,7 @@
         <v>22795</v>
       </c>
       <c r="C42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
@@ -1638,7 +1338,7 @@
         <v>22795</v>
       </c>
       <c r="G42" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H42" t="s">
         <v>1</v>
@@ -1655,7 +1355,7 @@
         <v>23206</v>
       </c>
       <c r="C43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
@@ -1667,13 +1367,13 @@
         <v>23206</v>
       </c>
       <c r="G43" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H43" t="s">
         <v>1</v>
       </c>
       <c r="I43" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44">
@@ -1689,20 +1389,8 @@
       <c r="D44" t="s">
         <v>1</v>
       </c>
-      <c r="E44" t="n">
-        <v>23532</v>
-      </c>
-      <c r="F44" t="n">
-        <v>23536</v>
-      </c>
-      <c r="G44" t="s">
-        <v>0</v>
-      </c>
-      <c r="H44" t="s">
-        <v>1</v>
-      </c>
-      <c r="I44" t="b">
-        <v>1</v>
+      <c r="E44" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1731,7 +1419,7 @@
         <v>1</v>
       </c>
       <c r="I45" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1742,7 +1430,7 @@
         <v>24259</v>
       </c>
       <c r="C46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
@@ -1754,7 +1442,7 @@
         <v>24259</v>
       </c>
       <c r="G46" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H46" t="s">
         <v>1</v>
@@ -1771,7 +1459,7 @@
         <v>24351</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
@@ -1783,7 +1471,7 @@
         <v>24351</v>
       </c>
       <c r="G47" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H47" t="s">
         <v>1</v>
@@ -1800,7 +1488,7 @@
         <v>25403</v>
       </c>
       <c r="C48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
@@ -1812,7 +1500,7 @@
         <v>25403</v>
       </c>
       <c r="G48" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H48" t="s">
         <v>1</v>
@@ -1829,7 +1517,7 @@
         <v>26177</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
@@ -1838,10 +1526,10 @@
         <v>26175</v>
       </c>
       <c r="F49" t="n">
-        <v>26177</v>
+        <v>26176</v>
       </c>
       <c r="G49" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="H49" t="s">
         <v>1</v>
@@ -1863,20 +1551,8 @@
       <c r="D50" t="s">
         <v>1</v>
       </c>
-      <c r="E50" t="n">
-        <v>26204</v>
-      </c>
-      <c r="F50" t="n">
-        <v>26208</v>
-      </c>
-      <c r="G50" t="s">
-        <v>0</v>
-      </c>
-      <c r="H50" t="s">
-        <v>1</v>
-      </c>
-      <c r="I50" t="b">
-        <v>1</v>
+      <c r="E50" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="51">
@@ -1887,25 +1563,13 @@
         <v>26678</v>
       </c>
       <c r="C51" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
       </c>
-      <c r="E51" t="n">
-        <v>26677</v>
-      </c>
-      <c r="F51" t="n">
-        <v>26678</v>
-      </c>
-      <c r="G51" t="s">
-        <v>23</v>
-      </c>
-      <c r="H51" t="s">
-        <v>1</v>
-      </c>
-      <c r="I51" t="b">
-        <v>1</v>
+      <c r="E51" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="52">
@@ -1916,19 +1580,19 @@
         <v>26885</v>
       </c>
       <c r="C52" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
       </c>
       <c r="E52" t="n">
-        <v>26883</v>
+        <v>26882</v>
       </c>
       <c r="F52" t="n">
         <v>26885</v>
       </c>
       <c r="G52" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="H52" t="s">
         <v>1</v>
@@ -1945,25 +1609,13 @@
         <v>26997</v>
       </c>
       <c r="C53" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
       </c>
-      <c r="E53" t="n">
-        <v>26995</v>
-      </c>
-      <c r="F53" t="n">
-        <v>26997</v>
-      </c>
-      <c r="G53" t="s">
-        <v>7</v>
-      </c>
-      <c r="H53" t="s">
-        <v>1</v>
-      </c>
-      <c r="I53" t="b">
-        <v>1</v>
+      <c r="E53" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="54">
@@ -1974,25 +1626,876 @@
         <v>27044</v>
       </c>
       <c r="C54" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
-      <c r="E54" t="n">
-        <v>27043</v>
-      </c>
-      <c r="F54" t="n">
-        <v>27044</v>
-      </c>
-      <c r="G54" t="s">
-        <v>14</v>
-      </c>
-      <c r="H54" t="s">
-        <v>1</v>
-      </c>
-      <c r="I54" t="b">
-        <v>1</v>
+      <c r="E54" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>77</v>
+      </c>
+      <c r="B55" t="n">
+        <v>79</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" t="n">
+        <v>77</v>
+      </c>
+      <c r="F55" t="n">
+        <v>79</v>
+      </c>
+      <c r="G55" t="s">
+        <v>7</v>
+      </c>
+      <c r="H55" t="s">
+        <v>1</v>
+      </c>
+      <c r="I55" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>214</v>
+      </c>
+      <c r="B56" t="n">
+        <v>216</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>341</v>
+      </c>
+      <c r="B57" t="n">
+        <v>343</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>505</v>
+      </c>
+      <c r="B58" t="n">
+        <v>507</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>889</v>
+      </c>
+      <c r="B59" t="n">
+        <v>891</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" t="n">
+        <v>889</v>
+      </c>
+      <c r="F59" t="n">
+        <v>891</v>
+      </c>
+      <c r="G59" t="s">
+        <v>12</v>
+      </c>
+      <c r="H59" t="s">
+        <v>1</v>
+      </c>
+      <c r="I59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>1199</v>
+      </c>
+      <c r="B60" t="n">
+        <v>1201</v>
+      </c>
+      <c r="C60" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60" t="n">
+        <v>1199</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1201</v>
+      </c>
+      <c r="G60" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" t="s">
+        <v>1</v>
+      </c>
+      <c r="I60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1205</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1206</v>
+      </c>
+      <c r="C61" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>2122</v>
+      </c>
+      <c r="B62" t="n">
+        <v>2126</v>
+      </c>
+      <c r="C62" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" t="n">
+        <v>2122</v>
+      </c>
+      <c r="F62" t="n">
+        <v>2126</v>
+      </c>
+      <c r="G62" t="s">
+        <v>0</v>
+      </c>
+      <c r="H62" t="s">
+        <v>1</v>
+      </c>
+      <c r="I62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>2656</v>
+      </c>
+      <c r="B63" t="n">
+        <v>2658</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" t="n">
+        <v>2656</v>
+      </c>
+      <c r="F63" t="n">
+        <v>2658</v>
+      </c>
+      <c r="G63" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" t="s">
+        <v>1</v>
+      </c>
+      <c r="I63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>2828</v>
+      </c>
+      <c r="B64" t="n">
+        <v>2830</v>
+      </c>
+      <c r="C64" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>2878</v>
+      </c>
+      <c r="B65" t="n">
+        <v>2880</v>
+      </c>
+      <c r="C65" t="s">
+        <v>8</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" t="n">
+        <v>2878</v>
+      </c>
+      <c r="F65" t="n">
+        <v>2880</v>
+      </c>
+      <c r="G65" t="s">
+        <v>8</v>
+      </c>
+      <c r="H65" t="s">
+        <v>1</v>
+      </c>
+      <c r="I65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3370</v>
+      </c>
+      <c r="B66" t="n">
+        <v>3372</v>
+      </c>
+      <c r="C66" t="s">
+        <v>8</v>
+      </c>
+      <c r="D66" t="s">
+        <v>1</v>
+      </c>
+      <c r="E66" t="n">
+        <v>3370</v>
+      </c>
+      <c r="F66" t="n">
+        <v>3372</v>
+      </c>
+      <c r="G66" t="s">
+        <v>8</v>
+      </c>
+      <c r="H66" t="s">
+        <v>1</v>
+      </c>
+      <c r="I66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>6331</v>
+      </c>
+      <c r="B67" t="n">
+        <v>6335</v>
+      </c>
+      <c r="C67" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" t="s">
+        <v>1</v>
+      </c>
+      <c r="E67" t="n">
+        <v>6331</v>
+      </c>
+      <c r="F67" t="n">
+        <v>6335</v>
+      </c>
+      <c r="G67" t="s">
+        <v>0</v>
+      </c>
+      <c r="H67" t="s">
+        <v>1</v>
+      </c>
+      <c r="I67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>6388</v>
+      </c>
+      <c r="B68" t="n">
+        <v>6391</v>
+      </c>
+      <c r="C68" t="s">
+        <v>6</v>
+      </c>
+      <c r="D68" t="s">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>6485</v>
+      </c>
+      <c r="B69" t="n">
+        <v>6487</v>
+      </c>
+      <c r="C69" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" t="s">
+        <v>1</v>
+      </c>
+      <c r="E69" t="n">
+        <v>6485</v>
+      </c>
+      <c r="F69" t="n">
+        <v>6487</v>
+      </c>
+      <c r="G69" t="s">
+        <v>8</v>
+      </c>
+      <c r="H69" t="s">
+        <v>1</v>
+      </c>
+      <c r="I69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>6978</v>
+      </c>
+      <c r="B70" t="n">
+        <v>6988</v>
+      </c>
+      <c r="C70" t="s">
+        <v>11</v>
+      </c>
+      <c r="D70" t="s">
+        <v>1</v>
+      </c>
+      <c r="E70" t="n">
+        <v>6978</v>
+      </c>
+      <c r="F70" t="n">
+        <v>6988</v>
+      </c>
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" t="s">
+        <v>1</v>
+      </c>
+      <c r="I70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>7108</v>
+      </c>
+      <c r="B71" t="n">
+        <v>7110</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>1</v>
+      </c>
+      <c r="E71" t="n">
+        <v>7108</v>
+      </c>
+      <c r="F71" t="n">
+        <v>7109</v>
+      </c>
+      <c r="G71" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" t="s">
+        <v>1</v>
+      </c>
+      <c r="I71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>7467</v>
+      </c>
+      <c r="B72" t="n">
+        <v>7470</v>
+      </c>
+      <c r="C72" t="s">
+        <v>27</v>
+      </c>
+      <c r="D72" t="s">
+        <v>1</v>
+      </c>
+      <c r="E72" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>3713</v>
+      </c>
+      <c r="B73" t="n">
+        <v>3717</v>
+      </c>
+      <c r="C73" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" t="s">
+        <v>1</v>
+      </c>
+      <c r="E73" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>3966</v>
+      </c>
+      <c r="B74" t="n">
+        <v>3967</v>
+      </c>
+      <c r="C74" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" t="s">
+        <v>1</v>
+      </c>
+      <c r="E74" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>3818</v>
+      </c>
+      <c r="B75" t="n">
+        <v>3820</v>
+      </c>
+      <c r="C75" t="s">
+        <v>8</v>
+      </c>
+      <c r="D75" t="s">
+        <v>1</v>
+      </c>
+      <c r="E75" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>3841</v>
+      </c>
+      <c r="B76" t="n">
+        <v>3843</v>
+      </c>
+      <c r="C76" t="s">
+        <v>8</v>
+      </c>
+      <c r="D76" t="s">
+        <v>1</v>
+      </c>
+      <c r="E76" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>6049</v>
+      </c>
+      <c r="B77" t="n">
+        <v>6051</v>
+      </c>
+      <c r="C77" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" t="s">
+        <v>1</v>
+      </c>
+      <c r="E77" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>6173</v>
+      </c>
+      <c r="B78" t="n">
+        <v>6177</v>
+      </c>
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>6990</v>
+      </c>
+      <c r="B79" t="n">
+        <v>6992</v>
+      </c>
+      <c r="C79" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" t="s">
+        <v>1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>7787</v>
+      </c>
+      <c r="B80" t="n">
+        <v>7789</v>
+      </c>
+      <c r="C80" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" t="s">
+        <v>1</v>
+      </c>
+      <c r="E80" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>7973</v>
+      </c>
+      <c r="B81" t="n">
+        <v>7976</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>7997</v>
+      </c>
+      <c r="B82" t="n">
+        <v>7998</v>
+      </c>
+      <c r="C82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" t="s">
+        <v>1</v>
+      </c>
+      <c r="E82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>10947</v>
+      </c>
+      <c r="B83" t="n">
+        <v>10949</v>
+      </c>
+      <c r="C83" t="s">
+        <v>8</v>
+      </c>
+      <c r="D83" t="s">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>10975</v>
+      </c>
+      <c r="B84" t="n">
+        <v>10979</v>
+      </c>
+      <c r="C84" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" t="s">
+        <v>1</v>
+      </c>
+      <c r="E84" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>12640</v>
+      </c>
+      <c r="B85" t="n">
+        <v>12642</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>13742</v>
+      </c>
+      <c r="B86" t="n">
+        <v>13744</v>
+      </c>
+      <c r="C86" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" t="s">
+        <v>1</v>
+      </c>
+      <c r="E86" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>13790</v>
+      </c>
+      <c r="B87" t="n">
+        <v>13791</v>
+      </c>
+      <c r="C87" t="s">
+        <v>16</v>
+      </c>
+      <c r="D87" t="s">
+        <v>1</v>
+      </c>
+      <c r="E87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>14053</v>
+      </c>
+      <c r="B88" t="n">
+        <v>14055</v>
+      </c>
+      <c r="C88" t="s">
+        <v>12</v>
+      </c>
+      <c r="D88" t="s">
+        <v>1</v>
+      </c>
+      <c r="E88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>14334</v>
+      </c>
+      <c r="B89" t="n">
+        <v>14335</v>
+      </c>
+      <c r="C89" t="s">
+        <v>25</v>
+      </c>
+      <c r="D89" t="s">
+        <v>1</v>
+      </c>
+      <c r="E89" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>14820</v>
+      </c>
+      <c r="B90" t="n">
+        <v>14822</v>
+      </c>
+      <c r="C90" t="s">
+        <v>12</v>
+      </c>
+      <c r="D90" t="s">
+        <v>1</v>
+      </c>
+      <c r="E90" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>15799</v>
+      </c>
+      <c r="B91" t="n">
+        <v>15801</v>
+      </c>
+      <c r="C91" t="s">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1</v>
+      </c>
+      <c r="E91" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>15854</v>
+      </c>
+      <c r="B92" t="n">
+        <v>15856</v>
+      </c>
+      <c r="C92" t="s">
+        <v>12</v>
+      </c>
+      <c r="D92" t="s">
+        <v>1</v>
+      </c>
+      <c r="E92" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>15988</v>
+      </c>
+      <c r="B93" t="n">
+        <v>15990</v>
+      </c>
+      <c r="C93" t="s">
+        <v>12</v>
+      </c>
+      <c r="D93" t="s">
+        <v>1</v>
+      </c>
+      <c r="E93" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>16461</v>
+      </c>
+      <c r="B94" t="n">
+        <v>16463</v>
+      </c>
+      <c r="C94" t="s">
+        <v>8</v>
+      </c>
+      <c r="D94" t="s">
+        <v>1</v>
+      </c>
+      <c r="E94" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>19907</v>
+      </c>
+      <c r="B95" t="n">
+        <v>19909</v>
+      </c>
+      <c r="C95" t="s">
+        <v>8</v>
+      </c>
+      <c r="D95" t="s">
+        <v>1</v>
+      </c>
+      <c r="E95" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>20887</v>
+      </c>
+      <c r="B96" t="n">
+        <v>20889</v>
+      </c>
+      <c r="C96" t="s">
+        <v>18</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>23620</v>
+      </c>
+      <c r="B97" t="n">
+        <v>23622</v>
+      </c>
+      <c r="C97" t="s">
+        <v>12</v>
+      </c>
+      <c r="D97" t="s">
+        <v>1</v>
+      </c>
+      <c r="E97" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Exercice Glozz : vers la fin. Reste :
- analyse du kappa
- production de l'excel
</commit_message>
<xml_diff>
--- a/master2/exoxml/devoir/out.xlsx
+++ b/master2/exoxml/devoir/out.xlsx
@@ -17,45 +17,60 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
+    <t>me</t>
+  </si>
+  <si>
+    <t>Mention</t>
+  </si>
+  <si>
+    <t>j'</t>
+  </si>
+  <si>
+    <t>missing annotation</t>
+  </si>
+  <si>
+    <t>Je</t>
+  </si>
+  <si>
+    <t>je</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
     <t>vous</t>
   </si>
   <si>
-    <t>Mention</t>
+    <t>J'</t>
+  </si>
+  <si>
+    <t>j</t>
   </si>
   <si>
     <t>Crainquebille</t>
   </si>
   <si>
+    <t>moi</t>
+  </si>
+  <si>
+    <t>Windreaver</t>
+  </si>
+  <si>
+    <t>ous</t>
+  </si>
+  <si>
     <t>votre</t>
   </si>
   <si>
     <t>mon</t>
   </si>
   <si>
-    <t>missing annotation</t>
-  </si>
-  <si>
-    <t>moi</t>
-  </si>
-  <si>
-    <t>me</t>
-  </si>
-  <si>
-    <t>je</t>
-  </si>
-  <si>
-    <t>j'</t>
+    <t>J</t>
   </si>
   <si>
     <t xml:space="preserve">vous </t>
   </si>
   <si>
-    <t>Windreaver</t>
-  </si>
-  <si>
-    <t>Je</t>
-  </si>
-  <si>
     <t>e</t>
   </si>
   <si>
@@ -65,12 +80,6 @@
     <t>tes</t>
   </si>
   <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
     <t>tu</t>
   </si>
   <si>
@@ -89,16 +98,7 @@
     <t>Moi</t>
   </si>
   <si>
-    <t>J'</t>
-  </si>
-  <si>
-    <t>J</t>
-  </si>
-  <si>
     <t xml:space="preserve"> je</t>
-  </si>
-  <si>
-    <t>ous</t>
   </si>
 </sst>
 </file>
@@ -443,10 +443,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>3460</v>
+        <v>77</v>
       </c>
       <c r="B1" t="n">
-        <v>3464</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -455,10 +455,10 @@
         <v>1</v>
       </c>
       <c r="E1" t="n">
-        <v>3460</v>
+        <v>77</v>
       </c>
       <c r="F1" t="n">
-        <v>3464</v>
+        <v>79</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
@@ -467,73 +467,49 @@
         <v>1</v>
       </c>
       <c r="I1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>4018</v>
+        <v>214</v>
       </c>
       <c r="B2" t="n">
-        <v>4022</v>
+        <v>216</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="n">
-        <v>4018</v>
-      </c>
-      <c r="F2" t="n">
-        <v>4022</v>
-      </c>
-      <c r="G2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="b">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>6034</v>
+        <v>341</v>
       </c>
       <c r="B3" t="n">
-        <v>6047</v>
+        <v>343</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" t="n">
-        <v>6034</v>
-      </c>
-      <c r="F3" t="n">
-        <v>6047</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I3" t="b">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>7220</v>
+        <v>505</v>
       </c>
       <c r="B4" t="n">
-        <v>7224</v>
+        <v>507</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -541,43 +517,31 @@
       <c r="D4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
-        <v>7220</v>
-      </c>
-      <c r="F4" t="n">
-        <v>7224</v>
-      </c>
-      <c r="G4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" t="b">
-        <v>0</v>
+      <c r="E4" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7642</v>
+        <v>889</v>
       </c>
       <c r="B5" t="n">
-        <v>7646</v>
+        <v>891</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
       </c>
       <c r="E5" t="n">
-        <v>7642</v>
+        <v>889</v>
       </c>
       <c r="F5" t="n">
-        <v>7646</v>
+        <v>891</v>
       </c>
       <c r="G5" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" t="s">
         <v>1</v>
@@ -588,25 +552,25 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>7677</v>
+        <v>1199</v>
       </c>
       <c r="B6" t="n">
-        <v>7682</v>
+        <v>1201</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
         <v>1</v>
       </c>
       <c r="E6" t="n">
-        <v>7677</v>
+        <v>1199</v>
       </c>
       <c r="F6" t="n">
-        <v>7682</v>
+        <v>1201</v>
       </c>
       <c r="G6" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" t="s">
         <v>1</v>
@@ -617,153 +581,189 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>7799</v>
+        <v>1205</v>
       </c>
       <c r="B7" t="n">
-        <v>7802</v>
+        <v>1206</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>11059</v>
+        <v>2122</v>
       </c>
       <c r="B8" t="n">
-        <v>11064</v>
+        <v>2126</v>
       </c>
       <c r="C8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>1</v>
       </c>
       <c r="E8" t="n">
-        <v>11059</v>
+        <v>2122</v>
       </c>
       <c r="F8" t="n">
-        <v>11064</v>
+        <v>2126</v>
       </c>
       <c r="G8" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="H8" t="s">
         <v>1</v>
       </c>
       <c r="I8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>12622</v>
+        <v>2656</v>
       </c>
       <c r="B9" t="n">
-        <v>12625</v>
+        <v>2658</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9" t="s">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
-        <v>5</v>
+      <c r="E9" t="n">
+        <v>2656</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2658</v>
+      </c>
+      <c r="G9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>12667</v>
+        <v>2828</v>
       </c>
       <c r="B10" t="n">
-        <v>12670</v>
+        <v>2830</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>15909</v>
+        <v>2878</v>
       </c>
       <c r="B11" t="n">
-        <v>15911</v>
+        <v>2880</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>5</v>
+      <c r="E11" t="n">
+        <v>2878</v>
+      </c>
+      <c r="F11" t="n">
+        <v>2880</v>
+      </c>
+      <c r="G11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>16984</v>
+        <v>3370</v>
       </c>
       <c r="B12" t="n">
-        <v>16988</v>
+        <v>3372</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E12" t="s">
-        <v>5</v>
+      <c r="E12" t="n">
+        <v>3370</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3372</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>17084</v>
+        <v>3460</v>
       </c>
       <c r="B13" t="n">
-        <v>17086</v>
+        <v>3464</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>1</v>
       </c>
       <c r="E13" t="n">
-        <v>17084</v>
+        <v>3460</v>
       </c>
       <c r="F13" t="n">
-        <v>17086</v>
+        <v>3464</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H13" t="s">
         <v>1</v>
       </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>17087</v>
+        <v>3713</v>
       </c>
       <c r="B14" t="n">
-        <v>17089</v>
+        <v>3717</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
@@ -772,173 +772,173 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>17245</v>
+        <v>3818</v>
       </c>
       <c r="B15" t="n">
-        <v>17247</v>
+        <v>3820</v>
       </c>
       <c r="C15" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D15" t="s">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>17296</v>
+        <v>3841</v>
       </c>
       <c r="B16" t="n">
-        <v>17301</v>
+        <v>3843</v>
       </c>
       <c r="C16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>17423</v>
+        <v>3966</v>
       </c>
       <c r="B17" t="n">
-        <v>17433</v>
+        <v>3967</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D17" t="s">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17795</v>
+        <v>4018</v>
       </c>
       <c r="B18" t="n">
-        <v>17799</v>
+        <v>4022</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>1</v>
       </c>
-      <c r="E18" t="s">
-        <v>5</v>
+      <c r="E18" t="n">
+        <v>4018</v>
+      </c>
+      <c r="F18" t="n">
+        <v>4022</v>
+      </c>
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18154</v>
+        <v>6034</v>
       </c>
       <c r="B19" t="n">
-        <v>18156</v>
+        <v>6047</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
       </c>
-      <c r="E19" t="s">
-        <v>5</v>
+      <c r="E19" t="n">
+        <v>6034</v>
+      </c>
+      <c r="F19" t="n">
+        <v>6047</v>
+      </c>
+      <c r="G19" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18739</v>
+        <v>6049</v>
       </c>
       <c r="B20" t="n">
-        <v>18741</v>
+        <v>6051</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D20" t="s">
         <v>1</v>
       </c>
-      <c r="E20" t="n">
-        <v>18740</v>
-      </c>
-      <c r="F20" t="n">
-        <v>18741</v>
-      </c>
-      <c r="G20" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" t="s">
-        <v>1</v>
-      </c>
-      <c r="I20" t="b">
-        <v>1</v>
+      <c r="E20" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19578</v>
+        <v>6173</v>
       </c>
       <c r="B21" t="n">
-        <v>19580</v>
+        <v>6177</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
         <v>1</v>
       </c>
-      <c r="E21" t="n">
-        <v>19578</v>
-      </c>
-      <c r="F21" t="n">
-        <v>19580</v>
-      </c>
-      <c r="G21" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" t="b">
-        <v>1</v>
+      <c r="E21" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19656</v>
+        <v>6331</v>
       </c>
       <c r="B22" t="n">
-        <v>19658</v>
+        <v>6335</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
         <v>1</v>
       </c>
       <c r="E22" t="n">
-        <v>19656</v>
+        <v>6331</v>
       </c>
       <c r="F22" t="n">
-        <v>19658</v>
+        <v>6335</v>
       </c>
       <c r="G22" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H22" t="s">
         <v>1</v>
@@ -949,761 +949,713 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>19670</v>
+        <v>6388</v>
       </c>
       <c r="B23" t="n">
-        <v>19683</v>
+        <v>6391</v>
       </c>
       <c r="C23" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
         <v>1</v>
       </c>
-      <c r="E23" t="n">
-        <v>19670</v>
-      </c>
-      <c r="F23" t="n">
-        <v>19683</v>
-      </c>
-      <c r="G23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" t="s">
-        <v>1</v>
-      </c>
-      <c r="I23" t="b">
-        <v>1</v>
+      <c r="E23" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>19829</v>
+        <v>6485</v>
       </c>
       <c r="B24" t="n">
-        <v>19832</v>
+        <v>6487</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
-        <v>5</v>
+      <c r="E24" t="n">
+        <v>6485</v>
+      </c>
+      <c r="F24" t="n">
+        <v>6487</v>
+      </c>
+      <c r="G24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>19910</v>
+        <v>6978</v>
       </c>
       <c r="B25" t="n">
-        <v>19912</v>
+        <v>6988</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D25" t="s">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
-        <v>5</v>
+      <c r="E25" t="n">
+        <v>6978</v>
+      </c>
+      <c r="F25" t="n">
+        <v>6988</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1</v>
+      </c>
+      <c r="I25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>19981</v>
+        <v>6990</v>
       </c>
       <c r="B26" t="n">
-        <v>19982</v>
+        <v>6992</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D26" t="s">
         <v>1</v>
       </c>
-      <c r="E26" t="s">
-        <v>5</v>
+      <c r="E26" t="n">
+        <v>6990</v>
+      </c>
+      <c r="F26" t="n">
+        <v>6992</v>
+      </c>
+      <c r="G26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>20030</v>
+        <v>7108</v>
       </c>
       <c r="B27" t="n">
-        <v>20031</v>
+        <v>7110</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="D27" t="s">
         <v>1</v>
       </c>
-      <c r="E27" t="s">
-        <v>5</v>
+      <c r="E27" t="n">
+        <v>7108</v>
+      </c>
+      <c r="F27" t="n">
+        <v>7109</v>
+      </c>
+      <c r="G27" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>20076</v>
+        <v>7220</v>
       </c>
       <c r="B28" t="n">
-        <v>20077</v>
+        <v>7224</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D28" t="s">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>5</v>
+      <c r="E28" t="n">
+        <v>7220</v>
+      </c>
+      <c r="F28" t="n">
+        <v>7224</v>
+      </c>
+      <c r="G28" t="s">
+        <v>7</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>20192</v>
+        <v>7467</v>
       </c>
       <c r="B29" t="n">
-        <v>20193</v>
+        <v>7470</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>20234</v>
+        <v>7642</v>
       </c>
       <c r="B30" t="n">
-        <v>20236</v>
+        <v>7646</v>
       </c>
       <c r="C30" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
-        <v>5</v>
+      <c r="E30" t="n">
+        <v>7642</v>
+      </c>
+      <c r="F30" t="n">
+        <v>7646</v>
+      </c>
+      <c r="G30" t="s">
+        <v>7</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>20289</v>
+        <v>7677</v>
       </c>
       <c r="B31" t="n">
-        <v>20290</v>
+        <v>7682</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
       </c>
-      <c r="E31" t="s">
-        <v>5</v>
+      <c r="E31" t="n">
+        <v>7677</v>
+      </c>
+      <c r="F31" t="n">
+        <v>7682</v>
+      </c>
+      <c r="G31" t="s">
+        <v>14</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>20351</v>
+        <v>7787</v>
       </c>
       <c r="B32" t="n">
-        <v>20353</v>
+        <v>7789</v>
       </c>
       <c r="C32" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
       </c>
-      <c r="E32" t="n">
-        <v>20351</v>
-      </c>
-      <c r="F32" t="n">
-        <v>20353</v>
-      </c>
-      <c r="G32" t="s">
-        <v>18</v>
-      </c>
-      <c r="H32" t="s">
-        <v>1</v>
-      </c>
-      <c r="I32" t="b">
-        <v>1</v>
+      <c r="E32" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>20462</v>
+        <v>7799</v>
       </c>
       <c r="B33" t="n">
-        <v>20464</v>
+        <v>7802</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>20541</v>
+        <v>7973</v>
       </c>
       <c r="B34" t="n">
-        <v>20543</v>
+        <v>7976</v>
       </c>
       <c r="C34" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>20602</v>
+        <v>7997</v>
       </c>
       <c r="B35" t="n">
-        <v>20604</v>
+        <v>7998</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
       </c>
-      <c r="E35" t="n">
-        <v>20602</v>
-      </c>
-      <c r="F35" t="n">
-        <v>20604</v>
-      </c>
-      <c r="G35" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" t="s">
-        <v>1</v>
-      </c>
-      <c r="I35" t="b">
-        <v>1</v>
+      <c r="E35" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>20967</v>
+        <v>10947</v>
       </c>
       <c r="B36" t="n">
-        <v>20969</v>
+        <v>10949</v>
       </c>
       <c r="C36" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
       </c>
-      <c r="E36" t="n">
-        <v>20967</v>
-      </c>
-      <c r="F36" t="n">
-        <v>20969</v>
-      </c>
-      <c r="G36" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" t="s">
-        <v>1</v>
-      </c>
-      <c r="I36" t="b">
-        <v>0</v>
+      <c r="E36" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>21116</v>
+        <v>10975</v>
       </c>
       <c r="B37" t="n">
-        <v>21119</v>
+        <v>10979</v>
       </c>
       <c r="C37" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>21260</v>
+        <v>11059</v>
       </c>
       <c r="B38" t="n">
-        <v>21264</v>
+        <v>11064</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
       </c>
-      <c r="E38" t="s">
-        <v>5</v>
+      <c r="E38" t="n">
+        <v>11059</v>
+      </c>
+      <c r="F38" t="n">
+        <v>11064</v>
+      </c>
+      <c r="G38" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" t="s">
+        <v>1</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>21819</v>
+        <v>12622</v>
       </c>
       <c r="B39" t="n">
-        <v>21823</v>
+        <v>12625</v>
       </c>
       <c r="C39" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>21895</v>
+        <v>12640</v>
       </c>
       <c r="B40" t="n">
-        <v>21899</v>
+        <v>12642</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>21942</v>
+        <v>12667</v>
       </c>
       <c r="B41" t="n">
-        <v>21945</v>
+        <v>12670</v>
       </c>
       <c r="C41" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>22793</v>
+        <v>13742</v>
       </c>
       <c r="B42" t="n">
-        <v>22795</v>
+        <v>13744</v>
       </c>
       <c r="C42" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
-      <c r="E42" t="n">
-        <v>22793</v>
-      </c>
-      <c r="F42" t="n">
-        <v>22795</v>
-      </c>
-      <c r="G42" t="s">
-        <v>8</v>
-      </c>
-      <c r="H42" t="s">
-        <v>1</v>
-      </c>
-      <c r="I42" t="b">
-        <v>1</v>
+      <c r="E42" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>23204</v>
+        <v>13790</v>
       </c>
       <c r="B43" t="n">
-        <v>23206</v>
+        <v>13791</v>
       </c>
       <c r="C43" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
       </c>
-      <c r="E43" t="n">
-        <v>23204</v>
-      </c>
-      <c r="F43" t="n">
-        <v>23206</v>
-      </c>
-      <c r="G43" t="s">
-        <v>12</v>
-      </c>
-      <c r="H43" t="s">
-        <v>1</v>
-      </c>
-      <c r="I43" t="b">
-        <v>0</v>
+      <c r="E43" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>23532</v>
+        <v>14053</v>
       </c>
       <c r="B44" t="n">
-        <v>23536</v>
+        <v>14055</v>
       </c>
       <c r="C44" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>23969</v>
+        <v>14334</v>
       </c>
       <c r="B45" t="n">
-        <v>23973</v>
+        <v>14335</v>
       </c>
       <c r="C45" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D45" t="s">
         <v>1</v>
       </c>
-      <c r="E45" t="n">
-        <v>23969</v>
-      </c>
-      <c r="F45" t="n">
-        <v>23973</v>
-      </c>
-      <c r="G45" t="s">
-        <v>0</v>
-      </c>
-      <c r="H45" t="s">
-        <v>1</v>
-      </c>
-      <c r="I45" t="b">
-        <v>0</v>
+      <c r="E45" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>24257</v>
+        <v>14820</v>
       </c>
       <c r="B46" t="n">
-        <v>24259</v>
+        <v>14822</v>
       </c>
       <c r="C46" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D46" t="s">
         <v>1</v>
       </c>
-      <c r="E46" t="n">
-        <v>24257</v>
-      </c>
-      <c r="F46" t="n">
-        <v>24259</v>
-      </c>
-      <c r="G46" t="s">
-        <v>8</v>
-      </c>
-      <c r="H46" t="s">
-        <v>1</v>
-      </c>
-      <c r="I46" t="b">
-        <v>1</v>
+      <c r="E46" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>24349</v>
+        <v>15799</v>
       </c>
       <c r="B47" t="n">
-        <v>24351</v>
+        <v>15801</v>
       </c>
       <c r="C47" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
-      <c r="E47" t="n">
-        <v>24349</v>
-      </c>
-      <c r="F47" t="n">
-        <v>24351</v>
-      </c>
-      <c r="G47" t="s">
-        <v>8</v>
-      </c>
-      <c r="H47" t="s">
-        <v>1</v>
-      </c>
-      <c r="I47" t="b">
-        <v>1</v>
+      <c r="E47" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>25401</v>
+        <v>15854</v>
       </c>
       <c r="B48" t="n">
-        <v>25403</v>
+        <v>15856</v>
       </c>
       <c r="C48" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
       </c>
-      <c r="E48" t="n">
-        <v>25401</v>
-      </c>
-      <c r="F48" t="n">
-        <v>25403</v>
-      </c>
-      <c r="G48" t="s">
-        <v>12</v>
-      </c>
-      <c r="H48" t="s">
-        <v>1</v>
-      </c>
-      <c r="I48" t="b">
-        <v>1</v>
+      <c r="E48" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>26175</v>
+        <v>15909</v>
       </c>
       <c r="B49" t="n">
-        <v>26177</v>
+        <v>15911</v>
       </c>
       <c r="C49" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
-      <c r="E49" t="n">
-        <v>26175</v>
-      </c>
-      <c r="F49" t="n">
-        <v>26176</v>
-      </c>
-      <c r="G49" t="s">
-        <v>25</v>
-      </c>
-      <c r="H49" t="s">
-        <v>1</v>
-      </c>
-      <c r="I49" t="b">
-        <v>1</v>
+      <c r="E49" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>26204</v>
+        <v>15988</v>
       </c>
       <c r="B50" t="n">
-        <v>26208</v>
+        <v>15990</v>
       </c>
       <c r="C50" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>26677</v>
+        <v>16461</v>
       </c>
       <c r="B51" t="n">
-        <v>26678</v>
+        <v>16463</v>
       </c>
       <c r="C51" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
       </c>
       <c r="E51" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>26883</v>
+        <v>16984</v>
       </c>
       <c r="B52" t="n">
-        <v>26885</v>
+        <v>16988</v>
       </c>
       <c r="C52" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D52" t="s">
         <v>1</v>
       </c>
-      <c r="E52" t="n">
-        <v>26882</v>
-      </c>
-      <c r="F52" t="n">
-        <v>26885</v>
-      </c>
-      <c r="G52" t="s">
-        <v>26</v>
-      </c>
-      <c r="H52" t="s">
-        <v>1</v>
-      </c>
-      <c r="I52" t="b">
-        <v>1</v>
+      <c r="E52" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>26995</v>
+        <v>17084</v>
       </c>
       <c r="B53" t="n">
-        <v>26997</v>
+        <v>17086</v>
       </c>
       <c r="C53" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D53" t="s">
         <v>1</v>
       </c>
-      <c r="E53" t="s">
-        <v>5</v>
+      <c r="E53" t="n">
+        <v>17084</v>
+      </c>
+      <c r="F53" t="n">
+        <v>17086</v>
+      </c>
+      <c r="G53" t="s">
+        <v>5</v>
+      </c>
+      <c r="H53" t="s">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>27043</v>
+        <v>17087</v>
       </c>
       <c r="B54" t="n">
-        <v>27044</v>
+        <v>17089</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D54" t="s">
         <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>77</v>
+        <v>17245</v>
       </c>
       <c r="B55" t="n">
-        <v>79</v>
+        <v>17247</v>
       </c>
       <c r="C55" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D55" t="s">
         <v>1</v>
       </c>
-      <c r="E55" t="n">
-        <v>77</v>
-      </c>
-      <c r="F55" t="n">
-        <v>79</v>
-      </c>
-      <c r="G55" t="s">
-        <v>7</v>
-      </c>
-      <c r="H55" t="s">
-        <v>1</v>
-      </c>
-      <c r="I55" t="b">
-        <v>1</v>
+      <c r="E55" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>214</v>
+        <v>17296</v>
       </c>
       <c r="B56" t="n">
-        <v>216</v>
+        <v>17301</v>
       </c>
       <c r="C56" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D56" t="s">
         <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>341</v>
+        <v>17423</v>
       </c>
       <c r="B57" t="n">
-        <v>343</v>
+        <v>17433</v>
       </c>
       <c r="C57" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D57" t="s">
         <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>505</v>
+        <v>17795</v>
       </c>
       <c r="B58" t="n">
-        <v>507</v>
+        <v>17799</v>
       </c>
       <c r="C58" t="s">
         <v>7</v>
@@ -1712,105 +1664,105 @@
         <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>889</v>
+        <v>18154</v>
       </c>
       <c r="B59" t="n">
-        <v>891</v>
+        <v>18156</v>
       </c>
       <c r="C59" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D59" t="s">
         <v>1</v>
       </c>
-      <c r="E59" t="n">
-        <v>889</v>
-      </c>
-      <c r="F59" t="n">
-        <v>891</v>
-      </c>
-      <c r="G59" t="s">
-        <v>12</v>
-      </c>
-      <c r="H59" t="s">
-        <v>1</v>
-      </c>
-      <c r="I59" t="b">
-        <v>0</v>
+      <c r="E59" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1199</v>
+        <v>18739</v>
       </c>
       <c r="B60" t="n">
-        <v>1201</v>
+        <v>18741</v>
       </c>
       <c r="C60" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D60" t="s">
         <v>1</v>
       </c>
       <c r="E60" t="n">
-        <v>1199</v>
+        <v>18740</v>
       </c>
       <c r="F60" t="n">
-        <v>1201</v>
+        <v>18741</v>
       </c>
       <c r="G60" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="H60" t="s">
         <v>1</v>
       </c>
       <c r="I60" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1205</v>
+        <v>19578</v>
       </c>
       <c r="B61" t="n">
-        <v>1206</v>
+        <v>19580</v>
       </c>
       <c r="C61" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D61" t="s">
         <v>1</v>
       </c>
-      <c r="E61" t="s">
-        <v>5</v>
+      <c r="E61" t="n">
+        <v>19578</v>
+      </c>
+      <c r="F61" t="n">
+        <v>19580</v>
+      </c>
+      <c r="G61" t="s">
+        <v>4</v>
+      </c>
+      <c r="H61" t="s">
+        <v>1</v>
+      </c>
+      <c r="I61" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2122</v>
+        <v>19656</v>
       </c>
       <c r="B62" t="n">
-        <v>2126</v>
+        <v>19658</v>
       </c>
       <c r="C62" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="D62" t="s">
         <v>1</v>
       </c>
       <c r="E62" t="n">
-        <v>2122</v>
+        <v>19656</v>
       </c>
       <c r="F62" t="n">
-        <v>2126</v>
+        <v>19658</v>
       </c>
       <c r="G62" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H62" t="s">
         <v>1</v>
@@ -1821,143 +1773,107 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2656</v>
+        <v>19670</v>
       </c>
       <c r="B63" t="n">
-        <v>2658</v>
+        <v>19683</v>
       </c>
       <c r="C63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D63" t="s">
         <v>1</v>
       </c>
       <c r="E63" t="n">
-        <v>2656</v>
+        <v>19670</v>
       </c>
       <c r="F63" t="n">
-        <v>2658</v>
+        <v>19683</v>
       </c>
       <c r="G63" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H63" t="s">
         <v>1</v>
       </c>
       <c r="I63" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2828</v>
+        <v>19829</v>
       </c>
       <c r="B64" t="n">
-        <v>2830</v>
+        <v>19832</v>
       </c>
       <c r="C64" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D64" t="s">
         <v>1</v>
       </c>
       <c r="E64" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2878</v>
+        <v>19907</v>
       </c>
       <c r="B65" t="n">
-        <v>2880</v>
+        <v>19909</v>
       </c>
       <c r="C65" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D65" t="s">
         <v>1</v>
       </c>
-      <c r="E65" t="n">
-        <v>2878</v>
-      </c>
-      <c r="F65" t="n">
-        <v>2880</v>
-      </c>
-      <c r="G65" t="s">
-        <v>8</v>
-      </c>
-      <c r="H65" t="s">
-        <v>1</v>
-      </c>
-      <c r="I65" t="b">
-        <v>0</v>
+      <c r="E65" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>3370</v>
+        <v>19910</v>
       </c>
       <c r="B66" t="n">
-        <v>3372</v>
+        <v>19912</v>
       </c>
       <c r="C66" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D66" t="s">
         <v>1</v>
       </c>
-      <c r="E66" t="n">
-        <v>3370</v>
-      </c>
-      <c r="F66" t="n">
-        <v>3372</v>
-      </c>
-      <c r="G66" t="s">
-        <v>8</v>
-      </c>
-      <c r="H66" t="s">
-        <v>1</v>
-      </c>
-      <c r="I66" t="b">
-        <v>1</v>
+      <c r="E66" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>6331</v>
+        <v>19981</v>
       </c>
       <c r="B67" t="n">
-        <v>6335</v>
+        <v>19982</v>
       </c>
       <c r="C67" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D67" t="s">
         <v>1</v>
       </c>
-      <c r="E67" t="n">
-        <v>6331</v>
-      </c>
-      <c r="F67" t="n">
-        <v>6335</v>
-      </c>
-      <c r="G67" t="s">
-        <v>0</v>
-      </c>
-      <c r="H67" t="s">
-        <v>1</v>
-      </c>
-      <c r="I67" t="b">
-        <v>1</v>
+      <c r="E67" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>6388</v>
+        <v>20030</v>
       </c>
       <c r="B68" t="n">
-        <v>6391</v>
+        <v>20031</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
@@ -1966,536 +1882,632 @@
         <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>6485</v>
+        <v>20076</v>
       </c>
       <c r="B69" t="n">
-        <v>6487</v>
+        <v>20077</v>
       </c>
       <c r="C69" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D69" t="s">
         <v>1</v>
       </c>
-      <c r="E69" t="n">
-        <v>6485</v>
-      </c>
-      <c r="F69" t="n">
-        <v>6487</v>
-      </c>
-      <c r="G69" t="s">
-        <v>8</v>
-      </c>
-      <c r="H69" t="s">
-        <v>1</v>
-      </c>
-      <c r="I69" t="b">
-        <v>0</v>
+      <c r="E69" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>6978</v>
+        <v>20192</v>
       </c>
       <c r="B70" t="n">
-        <v>6988</v>
+        <v>20193</v>
       </c>
       <c r="C70" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D70" t="s">
         <v>1</v>
       </c>
-      <c r="E70" t="n">
-        <v>6978</v>
-      </c>
-      <c r="F70" t="n">
-        <v>6988</v>
-      </c>
-      <c r="G70" t="s">
-        <v>11</v>
-      </c>
-      <c r="H70" t="s">
-        <v>1</v>
-      </c>
-      <c r="I70" t="b">
-        <v>0</v>
+      <c r="E70" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>7108</v>
+        <v>20234</v>
       </c>
       <c r="B71" t="n">
-        <v>7110</v>
+        <v>20236</v>
       </c>
       <c r="C71" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D71" t="s">
         <v>1</v>
       </c>
-      <c r="E71" t="n">
-        <v>7108</v>
-      </c>
-      <c r="F71" t="n">
-        <v>7109</v>
-      </c>
-      <c r="G71" t="s">
-        <v>16</v>
-      </c>
-      <c r="H71" t="s">
-        <v>1</v>
-      </c>
-      <c r="I71" t="b">
-        <v>0</v>
+      <c r="E71" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>7467</v>
+        <v>20289</v>
       </c>
       <c r="B72" t="n">
-        <v>7470</v>
+        <v>20290</v>
       </c>
       <c r="C72" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D72" t="s">
         <v>1</v>
       </c>
       <c r="E72" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>3713</v>
+        <v>20351</v>
       </c>
       <c r="B73" t="n">
-        <v>3717</v>
+        <v>20353</v>
       </c>
       <c r="C73" t="s">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D73" t="s">
         <v>1</v>
       </c>
-      <c r="E73" t="s">
-        <v>5</v>
+      <c r="E73" t="n">
+        <v>20351</v>
+      </c>
+      <c r="F73" t="n">
+        <v>20353</v>
+      </c>
+      <c r="G73" t="s">
+        <v>21</v>
+      </c>
+      <c r="H73" t="s">
+        <v>1</v>
+      </c>
+      <c r="I73" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>3966</v>
+        <v>20462</v>
       </c>
       <c r="B74" t="n">
-        <v>3967</v>
+        <v>20464</v>
       </c>
       <c r="C74" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D74" t="s">
         <v>1</v>
       </c>
       <c r="E74" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>3818</v>
+        <v>20541</v>
       </c>
       <c r="B75" t="n">
-        <v>3820</v>
+        <v>20543</v>
       </c>
       <c r="C75" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D75" t="s">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>3841</v>
+        <v>20602</v>
       </c>
       <c r="B76" t="n">
-        <v>3843</v>
+        <v>20604</v>
       </c>
       <c r="C76" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D76" t="s">
         <v>1</v>
       </c>
-      <c r="E76" t="s">
-        <v>5</v>
+      <c r="E76" t="n">
+        <v>20602</v>
+      </c>
+      <c r="F76" t="n">
+        <v>20604</v>
+      </c>
+      <c r="G76" t="s">
+        <v>4</v>
+      </c>
+      <c r="H76" t="s">
+        <v>1</v>
+      </c>
+      <c r="I76" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>6049</v>
+        <v>20887</v>
       </c>
       <c r="B77" t="n">
-        <v>6051</v>
+        <v>20889</v>
       </c>
       <c r="C77" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D77" t="s">
         <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>6173</v>
+        <v>20967</v>
       </c>
       <c r="B78" t="n">
-        <v>6177</v>
+        <v>20969</v>
       </c>
       <c r="C78" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" t="n">
+        <v>20967</v>
+      </c>
+      <c r="F78" t="n">
+        <v>20969</v>
+      </c>
+      <c r="G78" t="s">
+        <v>5</v>
+      </c>
+      <c r="H78" t="s">
+        <v>1</v>
+      </c>
+      <c r="I78" t="b">
         <v>0</v>
-      </c>
-      <c r="D78" t="s">
-        <v>1</v>
-      </c>
-      <c r="E78" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>6990</v>
+        <v>21116</v>
       </c>
       <c r="B79" t="n">
-        <v>6992</v>
+        <v>21119</v>
       </c>
       <c r="C79" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D79" t="s">
         <v>1</v>
       </c>
       <c r="E79" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>7787</v>
+        <v>21260</v>
       </c>
       <c r="B80" t="n">
-        <v>7789</v>
+        <v>21264</v>
       </c>
       <c r="C80" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="D80" t="s">
         <v>1</v>
       </c>
       <c r="E80" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>7973</v>
+        <v>21819</v>
       </c>
       <c r="B81" t="n">
-        <v>7976</v>
+        <v>21823</v>
       </c>
       <c r="C81" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D81" t="s">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>7997</v>
+        <v>21895</v>
       </c>
       <c r="B82" t="n">
-        <v>7998</v>
+        <v>21899</v>
       </c>
       <c r="C82" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D82" t="s">
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>10947</v>
+        <v>21942</v>
       </c>
       <c r="B83" t="n">
-        <v>10949</v>
+        <v>21945</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="D83" t="s">
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>10975</v>
+        <v>22793</v>
       </c>
       <c r="B84" t="n">
-        <v>10979</v>
+        <v>22795</v>
       </c>
       <c r="C84" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D84" t="s">
         <v>1</v>
       </c>
-      <c r="E84" t="s">
-        <v>5</v>
+      <c r="E84" t="n">
+        <v>22793</v>
+      </c>
+      <c r="F84" t="n">
+        <v>22795</v>
+      </c>
+      <c r="G84" t="s">
+        <v>5</v>
+      </c>
+      <c r="H84" t="s">
+        <v>1</v>
+      </c>
+      <c r="I84" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>12640</v>
+        <v>23204</v>
       </c>
       <c r="B85" t="n">
-        <v>12642</v>
+        <v>23206</v>
       </c>
       <c r="C85" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D85" t="s">
         <v>1</v>
       </c>
-      <c r="E85" t="s">
-        <v>5</v>
+      <c r="E85" t="n">
+        <v>23204</v>
+      </c>
+      <c r="F85" t="n">
+        <v>23206</v>
+      </c>
+      <c r="G85" t="s">
+        <v>4</v>
+      </c>
+      <c r="H85" t="s">
+        <v>1</v>
+      </c>
+      <c r="I85" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>13742</v>
+        <v>23532</v>
       </c>
       <c r="B86" t="n">
-        <v>13744</v>
+        <v>23536</v>
       </c>
       <c r="C86" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D86" t="s">
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>13790</v>
+        <v>23620</v>
       </c>
       <c r="B87" t="n">
-        <v>13791</v>
+        <v>23622</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D87" t="s">
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>14053</v>
+        <v>23969</v>
       </c>
       <c r="B88" t="n">
-        <v>14055</v>
+        <v>23973</v>
       </c>
       <c r="C88" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
       </c>
-      <c r="E88" t="s">
-        <v>5</v>
+      <c r="E88" t="n">
+        <v>23969</v>
+      </c>
+      <c r="F88" t="n">
+        <v>23973</v>
+      </c>
+      <c r="G88" t="s">
+        <v>7</v>
+      </c>
+      <c r="H88" t="s">
+        <v>1</v>
+      </c>
+      <c r="I88" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>14334</v>
+        <v>24257</v>
       </c>
       <c r="B89" t="n">
-        <v>14335</v>
+        <v>24259</v>
       </c>
       <c r="C89" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="D89" t="s">
         <v>1</v>
       </c>
-      <c r="E89" t="s">
-        <v>5</v>
+      <c r="E89" t="n">
+        <v>24257</v>
+      </c>
+      <c r="F89" t="n">
+        <v>24259</v>
+      </c>
+      <c r="G89" t="s">
+        <v>5</v>
+      </c>
+      <c r="H89" t="s">
+        <v>1</v>
+      </c>
+      <c r="I89" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>14820</v>
+        <v>24349</v>
       </c>
       <c r="B90" t="n">
-        <v>14822</v>
+        <v>24351</v>
       </c>
       <c r="C90" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="D90" t="s">
         <v>1</v>
       </c>
-      <c r="E90" t="s">
-        <v>5</v>
+      <c r="E90" t="n">
+        <v>24349</v>
+      </c>
+      <c r="F90" t="n">
+        <v>24351</v>
+      </c>
+      <c r="G90" t="s">
+        <v>5</v>
+      </c>
+      <c r="H90" t="s">
+        <v>1</v>
+      </c>
+      <c r="I90" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>15799</v>
+        <v>25401</v>
       </c>
       <c r="B91" t="n">
-        <v>15801</v>
+        <v>25403</v>
       </c>
       <c r="C91" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D91" t="s">
         <v>1</v>
       </c>
-      <c r="E91" t="s">
-        <v>5</v>
+      <c r="E91" t="n">
+        <v>25401</v>
+      </c>
+      <c r="F91" t="n">
+        <v>25403</v>
+      </c>
+      <c r="G91" t="s">
+        <v>4</v>
+      </c>
+      <c r="H91" t="s">
+        <v>1</v>
+      </c>
+      <c r="I91" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>15854</v>
+        <v>26175</v>
       </c>
       <c r="B92" t="n">
-        <v>15856</v>
+        <v>26177</v>
       </c>
       <c r="C92" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D92" t="s">
         <v>1</v>
       </c>
-      <c r="E92" t="s">
-        <v>5</v>
+      <c r="E92" t="n">
+        <v>26175</v>
+      </c>
+      <c r="F92" t="n">
+        <v>26176</v>
+      </c>
+      <c r="G92" t="s">
+        <v>16</v>
+      </c>
+      <c r="H92" t="s">
+        <v>1</v>
+      </c>
+      <c r="I92" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>15988</v>
+        <v>26204</v>
       </c>
       <c r="B93" t="n">
-        <v>15990</v>
+        <v>26208</v>
       </c>
       <c r="C93" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>16461</v>
+        <v>26677</v>
       </c>
       <c r="B94" t="n">
-        <v>16463</v>
+        <v>26678</v>
       </c>
       <c r="C94" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D94" t="s">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>19907</v>
+        <v>26883</v>
       </c>
       <c r="B95" t="n">
-        <v>19909</v>
+        <v>26885</v>
       </c>
       <c r="C95" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D95" t="s">
         <v>1</v>
       </c>
-      <c r="E95" t="s">
-        <v>5</v>
+      <c r="E95" t="n">
+        <v>26882</v>
+      </c>
+      <c r="F95" t="n">
+        <v>26885</v>
+      </c>
+      <c r="G95" t="s">
+        <v>27</v>
+      </c>
+      <c r="H95" t="s">
+        <v>1</v>
+      </c>
+      <c r="I95" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>20887</v>
+        <v>26995</v>
       </c>
       <c r="B96" t="n">
-        <v>20889</v>
+        <v>26997</v>
       </c>
       <c r="C96" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D96" t="s">
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>23620</v>
+        <v>27043</v>
       </c>
       <c r="B97" t="n">
-        <v>23622</v>
+        <v>27044</v>
       </c>
       <c r="C97" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D97" t="s">
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>